<commit_message>
Highlight selected MIGS and remove highlight when deselected
</commit_message>
<xml_diff>
--- a/files/MyRGC2022.xlsx
+++ b/files/MyRGC2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\percym\OneDrive\Documents\Education\myprojects\rgc\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9741FD51-9364-48DB-AA3B-1D700E6F405F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5924BA6A-F37A-4DAD-AB38-73617D8C96C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{FB88D2B2-9CD7-424F-9B37-793E627EACA7}"/>
   </bookViews>
@@ -1017,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4BB187-71F0-430A-9F07-6C3AA2400D21}">
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1212,10 +1212,10 @@
         <v>76</v>
       </c>
       <c r="I4" s="36">
-        <v>200</v>
+        <v>77</v>
       </c>
       <c r="J4" s="36">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="K4" s="36">
         <v>200</v>
@@ -1231,11 +1231,11 @@
       <c r="P4" s="39"/>
       <c r="Q4" s="40">
         <f>SUMPRODUCT(SMALL((B4,C4,D4,F4,H4,I4,K4,M4),{1;2;3;4;5;6}))</f>
-        <v>594</v>
+        <v>471</v>
       </c>
       <c r="R4" s="41">
         <f>SUMPRODUCT(LARGE((E4,G4,J4,N4),{1;2;3}))</f>
-        <v>59</v>
+        <v>259</v>
       </c>
       <c r="S4" s="42"/>
     </row>
@@ -1265,10 +1265,10 @@
         <v>74</v>
       </c>
       <c r="I5" s="36">
-        <v>200</v>
+        <v>73</v>
       </c>
       <c r="J5" s="36">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K5" s="36">
         <v>200</v>
@@ -1284,11 +1284,11 @@
       <c r="P5" s="39"/>
       <c r="Q5" s="40">
         <f>SUMPRODUCT(SMALL((B5,C5,D5,F5,H5,I5,K5,M5),{1;2;3;4;5;6}))</f>
-        <v>595</v>
+        <v>468</v>
       </c>
       <c r="R5" s="41">
         <f>SUMPRODUCT(LARGE((E5,G5,J5,N5),{1;2;3}))</f>
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="S5" s="42"/>
     </row>
@@ -1318,7 +1318,7 @@
         <v>82</v>
       </c>
       <c r="I6" s="36">
-        <v>200</v>
+        <v>77</v>
       </c>
       <c r="J6" s="36">
         <v>0</v>
@@ -1337,7 +1337,7 @@
       <c r="P6" s="39"/>
       <c r="Q6" s="40">
         <f>SUMPRODUCT(SMALL((B6,C6,D6,F6,H6,I6,K6,M6),{1;2;3;4;5;6}))</f>
-        <v>597</v>
+        <v>474</v>
       </c>
       <c r="R6" s="41">
         <f>SUMPRODUCT(LARGE((E6,G6,J6,N6),{1;2;3}))</f>
@@ -1371,10 +1371,10 @@
         <v>87</v>
       </c>
       <c r="I7" s="36">
-        <v>200</v>
+        <v>78</v>
       </c>
       <c r="J7" s="36">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="K7" s="36">
         <v>200</v>
@@ -1390,11 +1390,11 @@
       <c r="P7" s="39"/>
       <c r="Q7" s="40">
         <f>SUMPRODUCT(SMALL((B7,C7,D7,F7,H7,I7,K7,M7),{1;2;3;4;5;6}))</f>
-        <v>598</v>
+        <v>476</v>
       </c>
       <c r="R7" s="41">
         <f>SUMPRODUCT(LARGE((E7,G7,J7,N7),{1;2;3}))</f>
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="S7" s="42"/>
     </row>
@@ -1424,10 +1424,10 @@
         <v>85</v>
       </c>
       <c r="I8" s="36">
-        <v>200</v>
+        <v>77</v>
       </c>
       <c r="J8" s="36">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="K8" s="36">
         <v>200</v>
@@ -1443,11 +1443,11 @@
       <c r="P8" s="39"/>
       <c r="Q8" s="40">
         <f>SUMPRODUCT(SMALL((B8,C8,D8,F8,H8,I8,K8,M8),{1;2;3;4;5;6}))</f>
-        <v>601</v>
+        <v>478</v>
       </c>
       <c r="R8" s="41">
         <f>SUMPRODUCT(LARGE((E8,G8,J8,N8),{1;2;3}))</f>
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="S8" s="42"/>
     </row>
@@ -1477,10 +1477,10 @@
         <v>79</v>
       </c>
       <c r="I9" s="36">
-        <v>200</v>
+        <v>77</v>
       </c>
       <c r="J9" s="36">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="K9" s="36">
         <v>200</v>
@@ -1496,11 +1496,11 @@
       <c r="P9" s="39"/>
       <c r="Q9" s="40">
         <f>SUMPRODUCT(SMALL((B9,C9,D9,F9,H9,I9,K9,M9),{1;2;3;4;5;6}))</f>
-        <v>603</v>
+        <v>480</v>
       </c>
       <c r="R9" s="41">
         <f>SUMPRODUCT(LARGE((E9,G9,J9,N9),{1;2;3}))</f>
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="S9" s="42"/>
     </row>
@@ -1530,10 +1530,10 @@
         <v>83</v>
       </c>
       <c r="I10" s="36">
-        <v>200</v>
+        <v>75</v>
       </c>
       <c r="J10" s="36">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K10" s="36">
         <v>200</v>
@@ -1549,11 +1549,11 @@
       <c r="P10" s="39"/>
       <c r="Q10" s="40">
         <f>SUMPRODUCT(SMALL((B10,C10,D10,F10,H10,I10,K10,M10),{1;2;3;4;5;6}))</f>
-        <v>629</v>
+        <v>504</v>
       </c>
       <c r="R10" s="41">
         <f>SUMPRODUCT(LARGE((E10,G10,J10,N10),{1;2;3}))</f>
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="S10" s="42"/>
     </row>
@@ -1583,10 +1583,10 @@
         <v>89</v>
       </c>
       <c r="I11" s="36">
-        <v>200</v>
+        <v>78</v>
       </c>
       <c r="J11" s="36">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="K11" s="36">
         <v>200</v>
@@ -1602,11 +1602,11 @@
       <c r="P11" s="39"/>
       <c r="Q11" s="40">
         <f>SUMPRODUCT(SMALL((B11,C11,D11,F11,H11,I11,K11,M11),{1;2;3;4;5;6}))</f>
-        <v>635</v>
+        <v>513</v>
       </c>
       <c r="R11" s="41">
         <f>SUMPRODUCT(LARGE((E11,G11,J11,N11),{1;2;3}))</f>
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="S11" s="42"/>
     </row>
@@ -1636,10 +1636,10 @@
         <v>79</v>
       </c>
       <c r="I12" s="36">
-        <v>200</v>
+        <v>89</v>
       </c>
       <c r="J12" s="36">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="K12" s="36">
         <v>200</v>
@@ -1655,11 +1655,11 @@
       <c r="P12" s="39"/>
       <c r="Q12" s="40">
         <f>SUMPRODUCT(SMALL((B12,C12,D12,F12,H12,I12,K12,M12),{1;2;3;4;5;6}))</f>
-        <v>710</v>
+        <v>599</v>
       </c>
       <c r="R12" s="41">
         <f>SUMPRODUCT(LARGE((E12,G12,J12,N12),{1;2;3}))</f>
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="S12" s="42"/>
     </row>
@@ -1689,10 +1689,10 @@
         <v>80</v>
       </c>
       <c r="I13" s="36">
-        <v>200</v>
+        <v>77</v>
       </c>
       <c r="J13" s="36">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="K13" s="36">
         <v>200</v>
@@ -1708,11 +1708,11 @@
       <c r="P13" s="39"/>
       <c r="Q13" s="40">
         <f>SUMPRODUCT(SMALL((B13,C13,D13,F13,H13,I13,K13,M13),{1;2;3;4;5;6}))</f>
-        <v>720</v>
+        <v>597</v>
       </c>
       <c r="R13" s="41">
         <f>SUMPRODUCT(LARGE((E13,G13,J13,N13),{1;2;3}))</f>
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="S13" s="42"/>
     </row>
@@ -1742,10 +1742,10 @@
         <v>73</v>
       </c>
       <c r="I14" s="36">
-        <v>200</v>
+        <v>78</v>
       </c>
       <c r="J14" s="36">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K14" s="36">
         <v>200</v>
@@ -1761,11 +1761,11 @@
       <c r="P14" s="39"/>
       <c r="Q14" s="40">
         <f>SUMPRODUCT(SMALL((B14,C14,D14,F14,H14,I14,K14,M14),{1;2;3;4;5;6}))</f>
-        <v>727</v>
+        <v>605</v>
       </c>
       <c r="R14" s="41">
         <f>SUMPRODUCT(LARGE((E14,G14,J14,N14),{1;2;3}))</f>
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="S14" s="42"/>
     </row>
@@ -1848,7 +1848,7 @@
         <v>200</v>
       </c>
       <c r="I16" s="36">
-        <v>200</v>
+        <v>85</v>
       </c>
       <c r="J16" s="36">
         <v>0</v>
@@ -1867,7 +1867,7 @@
       <c r="P16" s="39"/>
       <c r="Q16" s="40">
         <f>SUMPRODUCT(SMALL((B16,C16,D16,F16,H16,I16,K16,M16),{1;2;3;4;5;6}))</f>
-        <v>731</v>
+        <v>616</v>
       </c>
       <c r="R16" s="41">
         <f>SUMPRODUCT(LARGE((E16,G16,J16,N16),{1;2;3}))</f>
@@ -1901,10 +1901,10 @@
         <v>83</v>
       </c>
       <c r="I17" s="36">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="J17" s="36">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="K17" s="36">
         <v>200</v>
@@ -1920,11 +1920,11 @@
       <c r="P17" s="39"/>
       <c r="Q17" s="40">
         <f>SUMPRODUCT(SMALL((B17,C17,D17,F17,H17,I17,K17,M17),{1;2;3;4;5;6}))</f>
-        <v>737</v>
+        <v>617</v>
       </c>
       <c r="R17" s="41">
         <f>SUMPRODUCT(LARGE((E17,G17,J17,N17),{1;2;3}))</f>
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="S17" s="42"/>
     </row>
@@ -1954,7 +1954,7 @@
         <v>88</v>
       </c>
       <c r="I18" s="36">
-        <v>200</v>
+        <v>81</v>
       </c>
       <c r="J18" s="36">
         <v>0</v>
@@ -1973,7 +1973,7 @@
       <c r="P18" s="39"/>
       <c r="Q18" s="40">
         <f>SUMPRODUCT(SMALL((B18,C18,D18,F18,H18,I18,K18,M18),{1;2;3;4;5;6}))</f>
-        <v>748</v>
+        <v>629</v>
       </c>
       <c r="R18" s="41">
         <f>SUMPRODUCT(LARGE((E18,G18,J18,N18),{1;2;3}))</f>
@@ -2007,7 +2007,7 @@
         <v>87</v>
       </c>
       <c r="I19" s="36">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="J19" s="36">
         <v>0</v>
@@ -2026,7 +2026,7 @@
       <c r="P19" s="39"/>
       <c r="Q19" s="40">
         <f>SUMPRODUCT(SMALL((B19,C19,D19,F19,H19,I19,K19,M19),{1;2;3;4;5;6}))</f>
-        <v>837</v>
+        <v>717</v>
       </c>
       <c r="R19" s="41">
         <f>SUMPRODUCT(LARGE((E19,G19,J19,N19),{1;2;3}))</f>
@@ -2060,10 +2060,10 @@
         <v>85</v>
       </c>
       <c r="I20" s="36">
-        <v>200</v>
+        <v>78</v>
       </c>
       <c r="J20" s="36">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K20" s="36">
         <v>200</v>
@@ -2079,11 +2079,11 @@
       <c r="P20" s="39"/>
       <c r="Q20" s="40">
         <f>SUMPRODUCT(SMALL((B20,C20,D20,F20,H20,I20,K20,M20),{1;2;3;4;5;6}))</f>
-        <v>844</v>
+        <v>722</v>
       </c>
       <c r="R20" s="41">
         <f>SUMPRODUCT(LARGE((E20,G20,J20,N20),{1;2;3}))</f>
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="S20" s="42"/>
     </row>
@@ -2116,7 +2116,7 @@
         <v>200</v>
       </c>
       <c r="J21" s="36">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="K21" s="36">
         <v>200</v>
@@ -2136,7 +2136,7 @@
       </c>
       <c r="R21" s="41">
         <f>SUMPRODUCT(LARGE((E21,G21,J21,N21),{1;2;3}))</f>
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="S21" s="42"/>
     </row>
@@ -2166,10 +2166,10 @@
         <v>94</v>
       </c>
       <c r="I22" s="36">
-        <v>200</v>
+        <v>82</v>
       </c>
       <c r="J22" s="36">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="K22" s="36">
         <v>200</v>
@@ -2185,11 +2185,11 @@
       <c r="P22" s="39"/>
       <c r="Q22" s="40">
         <f>SUMPRODUCT(SMALL((B22,C22,D22,F22,H22,I22,K22,M22),{1;2;3;4;5;6}))</f>
-        <v>852</v>
+        <v>734</v>
       </c>
       <c r="R22" s="41">
         <f>SUMPRODUCT(LARGE((E22,G22,J22,N22),{1;2;3}))</f>
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="S22" s="42"/>
     </row>
@@ -2219,10 +2219,10 @@
         <v>77</v>
       </c>
       <c r="I23" s="36">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="J23" s="36">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="K23" s="36">
         <v>200</v>
@@ -2238,11 +2238,11 @@
       <c r="P23" s="39"/>
       <c r="Q23" s="40">
         <f>SUMPRODUCT(SMALL((B23,C23,D23,F23,H23,I23,K23,M23),{1;2;3;4;5;6}))</f>
-        <v>853</v>
+        <v>733</v>
       </c>
       <c r="R23" s="41">
         <f>SUMPRODUCT(LARGE((E23,G23,J23,N23),{1;2;3}))</f>
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="S23" s="42"/>
     </row>
@@ -2272,7 +2272,7 @@
         <v>93</v>
       </c>
       <c r="I24" s="36">
-        <v>200</v>
+        <v>79</v>
       </c>
       <c r="J24" s="36">
         <v>0</v>
@@ -2291,7 +2291,7 @@
       <c r="P24" s="39"/>
       <c r="Q24" s="40">
         <f>SUMPRODUCT(SMALL((B24,C24,D24,F24,H24,I24,K24,M24),{1;2;3;4;5;6}))</f>
-        <v>881</v>
+        <v>760</v>
       </c>
       <c r="R24" s="41">
         <f>SUMPRODUCT(LARGE((E24,G24,J24,N24),{1;2;3}))</f>
@@ -2328,7 +2328,7 @@
         <v>200</v>
       </c>
       <c r="J25" s="36">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="K25" s="36">
         <v>200</v>
@@ -2348,7 +2348,7 @@
       </c>
       <c r="R25" s="41">
         <f>SUMPRODUCT(LARGE((E25,G25,J25,N25),{1;2;3}))</f>
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="S25" s="42"/>
     </row>
@@ -2381,7 +2381,7 @@
         <v>200</v>
       </c>
       <c r="J26" s="36">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="K26" s="36">
         <v>200</v>
@@ -2401,7 +2401,7 @@
       </c>
       <c r="R26" s="41">
         <f>SUMPRODUCT(LARGE((E26,G26,J26,N26),{1;2;3}))</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="S26" s="42"/>
     </row>
@@ -2484,7 +2484,7 @@
         <v>200</v>
       </c>
       <c r="I28" s="36">
-        <v>200</v>
+        <v>89</v>
       </c>
       <c r="J28" s="36">
         <v>0</v>
@@ -2503,7 +2503,7 @@
       <c r="P28" s="39"/>
       <c r="Q28" s="40">
         <f>SUMPRODUCT(SMALL((B28,C28,D28,F28,H28,I28,K28,M28),{1;2;3;4;5;6}))</f>
-        <v>961</v>
+        <v>850</v>
       </c>
       <c r="R28" s="41">
         <f>SUMPRODUCT(LARGE((E28,G28,J28,N28),{1;2;3}))</f>
@@ -2643,10 +2643,10 @@
         <v>86</v>
       </c>
       <c r="I31" s="36">
-        <v>200</v>
+        <v>81</v>
       </c>
       <c r="J31" s="36">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="K31" s="36">
         <v>200</v>
@@ -2662,11 +2662,11 @@
       <c r="P31" s="39"/>
       <c r="Q31" s="40">
         <f>SUMPRODUCT(SMALL((B31,C31,D31,F31,H31,I31,K31,M31),{1;2;3;4;5;6}))</f>
-        <v>974</v>
+        <v>855</v>
       </c>
       <c r="R31" s="41">
         <f>SUMPRODUCT(LARGE((E31,G31,J31,N31),{1;2;3}))</f>
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="S31" s="42"/>
     </row>
@@ -2699,7 +2699,7 @@
         <v>200</v>
       </c>
       <c r="J32" s="36">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K32" s="36">
         <v>200</v>
@@ -2719,7 +2719,7 @@
       </c>
       <c r="R32" s="41">
         <f>SUMPRODUCT(LARGE((E32,G32,J32,N32),{1;2;3}))</f>
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="S32" s="42"/>
     </row>
@@ -2802,10 +2802,10 @@
         <v>200</v>
       </c>
       <c r="I34" s="36">
-        <v>200</v>
+        <v>75</v>
       </c>
       <c r="J34" s="36">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="K34" s="36">
         <v>200</v>
@@ -2821,11 +2821,11 @@
       <c r="P34" s="39"/>
       <c r="Q34" s="40">
         <f>SUMPRODUCT(SMALL((B34,C34,D34,F34,H34,I34,K34,M34),{1;2;3;4;5;6}))</f>
-        <v>1082</v>
+        <v>957</v>
       </c>
       <c r="R34" s="41">
         <f>SUMPRODUCT(LARGE((E34,G34,J34,N34),{1;2;3}))</f>
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="S34" s="42"/>
     </row>
@@ -2908,7 +2908,7 @@
         <v>200</v>
       </c>
       <c r="I36" s="36">
-        <v>200</v>
+        <v>82</v>
       </c>
       <c r="J36" s="36">
         <v>0</v>
@@ -2927,7 +2927,7 @@
       <c r="P36" s="39"/>
       <c r="Q36" s="40">
         <f>SUMPRODUCT(SMALL((B36,C36,D36,F36,H36,I36,K36,M36),{1;2;3;4;5;6}))</f>
-        <v>1091</v>
+        <v>973</v>
       </c>
       <c r="R36" s="41">
         <f>SUMPRODUCT(LARGE((E36,G36,J36,N36),{1;2;3}))</f>
@@ -2961,7 +2961,7 @@
         <v>200</v>
       </c>
       <c r="I37" s="36">
-        <v>200</v>
+        <v>101</v>
       </c>
       <c r="J37" s="36">
         <v>0</v>
@@ -2980,7 +2980,7 @@
       <c r="P37" s="39"/>
       <c r="Q37" s="40">
         <f>SUMPRODUCT(SMALL((B37,C37,D37,F37,H37,I37,K37,M37),{1;2;3;4;5;6}))</f>
-        <v>1095</v>
+        <v>996</v>
       </c>
       <c r="R37" s="41">
         <f>SUMPRODUCT(LARGE((E37,G37,J37,N37),{1;2;3}))</f>
@@ -3229,7 +3229,7 @@
         <v>200</v>
       </c>
       <c r="J42" s="36">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="K42" s="36">
         <v>200</v>
@@ -3249,7 +3249,7 @@
       </c>
       <c r="R42" s="41">
         <f>SUMPRODUCT(LARGE((E42,G42,J42,N42),{1;2;3}))</f>
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="S42" s="42"/>
     </row>
@@ -3332,7 +3332,7 @@
         <v>200</v>
       </c>
       <c r="I44" s="36">
-        <v>200</v>
+        <v>81</v>
       </c>
       <c r="J44" s="36">
         <v>0</v>
@@ -3351,7 +3351,7 @@
       <c r="P44" s="39"/>
       <c r="Q44" s="40">
         <f>SUMPRODUCT(SMALL((B44,C44,D44,F44,H44,I44,K44,M44),{1;2;3;4;5;6}))</f>
-        <v>1200</v>
+        <v>1081</v>
       </c>
       <c r="R44" s="41">
         <f>SUMPRODUCT(LARGE((E44,G44,J44,N44),{1;2;3}))</f>

</xml_diff>